<commit_message>
vault backup: 2024-10-24 14:05:16
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Internships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Documents\Notes\PPE\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2003C93-E93E-418C-B4FC-513097434455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC57E5-66D6-4BD2-A417-AFACCE813E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -668,21 +666,21 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -723,13 +721,13 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -747,13 +745,13 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F10" ca="1" si="0">C3-TODAY()</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -771,13 +769,13 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -795,13 +793,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -819,13 +817,13 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -843,13 +841,13 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -867,13 +865,13 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -891,13 +889,13 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -915,13 +913,13 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
vault backup: 2024-10-26 06:14:41
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Documents\Notes\PPE\Extra Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC57E5-66D6-4BD2-A417-AFACCE813E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE9337-22EC-4300-A019-1CB5E5A1BC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>Role</t>
   </si>
@@ -162,10 +162,46 @@
     <t>RBB Economics</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>https://www.rbbecon.com/careers</t>
+  </si>
+  <si>
+    <t>https://fca.wd3.myworkdayjobs.com/en-US/FCA_earlycareers/job/London/XMLNAME-2025-Economics-Graduate-Programme_JR0015990?jobFamily=4b24e5d1ad610154334083cd5b098f0f&amp;locations=4b24e5d1ad61016bb01cec6a9e095721&amp;locations=0efb24a735660101a9a87e4860b50000</t>
+  </si>
+  <si>
+    <t>https://fca.wd3.myworkdayjobs.com/en-US/FCA_earlycareers/job/Leeds/XMLNAME-2025-Leeds-Economics-Graduate-Programme_JR0016008?jobFamily=4b24e5d1ad610154334083cd5b098f0f&amp;locations=4b24e5d1ad61016bb01cec6a9e095721&amp;locations=0efb24a735660101a9a87e4860b50000</t>
+  </si>
+  <si>
+    <t>Economics Graduate</t>
+  </si>
+  <si>
+    <t>FCA</t>
+  </si>
+  <si>
+    <t>https://www.mottmac.com/en-gb/careers/explore-our-careers/2025-uk-graduate-place-economist-career-path-5099/</t>
+  </si>
+  <si>
+    <t>Economics Graduate Career Path</t>
+  </si>
+  <si>
+    <t>Mott MacDonald</t>
+  </si>
+  <si>
+    <t>https://carriere.talan.com/offre-emploi/detail/?tx_talansmartrecruitorconnector_pi1%5Bid%5D=744000017588760&amp;tx_talansmartrecruitorconnector_pi1%5Baction%5D=job&amp;tx_talansmartrecruitorconnector_pi1%5Bcontroller%5D=JobOffers&amp;cHash=e6d85c147b4d326f4ed93ee51be9aa10</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Talan</t>
+  </si>
+  <si>
+    <t>Economic Analyst</t>
+  </si>
+  <si>
+    <t>https://www.oxfordeconomics.com/vacancy/graduate-recruitment-2/</t>
+  </si>
+  <si>
+    <t>Oxford Economics</t>
   </si>
 </sst>
 </file>
@@ -663,24 +699,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB83AAD-773A-4D2C-A53F-9AF66BB57483}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -721,13 +757,13 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -744,14 +780,14 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" ca="1" si="0">C3-TODAY()</f>
-        <v>12</v>
+        <f t="shared" ref="F3:F16" ca="1" si="0">C3-TODAY()</f>
+        <v>8</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -769,13 +805,13 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -793,13 +829,13 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -817,13 +853,13 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -841,13 +877,13 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -865,13 +901,13 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -889,13 +925,13 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -913,29 +949,153 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
       <c r="G11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45607</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45607</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45607</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45607</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45607</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -977,6 +1137,11 @@
     <hyperlink ref="D9" r:id="rId8" xr:uid="{3E8E487D-D4F7-4A35-B9AE-8DA1FB6CC92E}"/>
     <hyperlink ref="D10" r:id="rId9" xr:uid="{7B6DF712-57ED-43EF-8361-E5AF1227004E}"/>
     <hyperlink ref="D11" r:id="rId10" xr:uid="{F376C21B-3E8F-45C1-9568-A2846A1DD305}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{01352256-C78F-4902-906C-EBCE4F586F92}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{862D000A-260F-40FF-9DE5-3984640192F5}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{DE809EF5-F9B9-46FF-8BE7-46E61D80A9D6}"/>
+    <hyperlink ref="D15" r:id="rId14" display="https://carriere.talan.com/offre-emploi/detail/?tx_talansmartrecruitorconnector_pi1%5Bid%5D=744000017588760&amp;tx_talansmartrecruitorconnector_pi1%5Baction%5D=job&amp;tx_talansmartrecruitorconnector_pi1%5Bcontroller%5D=JobOffers&amp;cHash=e6d85c147b4d326f4ed93ee51be9aa10" xr:uid="{E941F7B3-08E1-4FA5-BAF4-6DA62A0A82F7}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{824C8599-388D-47F0-A615-C4F85FD1051F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2024-10-29 21:38:27
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE9337-22EC-4300-A019-1CB5E5A1BC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD919A1-2608-4258-8E6F-E14592CFC76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -233,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +243,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -313,6 +319,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -702,7 +717,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,55 +772,55 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>45599</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F16" ca="1" si="0">C3-TODAY()</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="10">
         <v>45603</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
@@ -829,7 +844,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
@@ -853,7 +868,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
@@ -877,7 +892,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
@@ -901,33 +916,33 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>45592</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -949,7 +964,7 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
@@ -973,7 +988,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
@@ -997,7 +1012,7 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>29</v>
@@ -1021,7 +1036,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
@@ -1045,7 +1060,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>28</v>
@@ -1069,7 +1084,7 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>28</v>
@@ -1093,7 +1108,7 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
vault backup: 2024-11-04 11:53:15
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD919A1-2608-4258-8E6F-E14592CFC76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B20A07-66D5-4FE8-BD78-B5748ABD41CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Role</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Oxford Economics</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Cover Letter</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +255,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -328,6 +346,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -714,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB83AAD-773A-4D2C-A53F-9AF66BB57483}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,9 +761,10 @@
     <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,8 +786,11 @@
       <c r="G1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -772,13 +808,13 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -796,13 +832,13 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F16" ca="1" si="0">C3-TODAY()</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -820,37 +856,37 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="15">
         <v>45599</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -868,13 +904,13 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -892,13 +928,13 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -916,13 +952,13 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
@@ -940,13 +976,13 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -964,13 +1000,13 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -988,85 +1024,88 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="18">
         <v>45607</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="10">
         <v>45607</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>45607</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -1084,13 +1123,13 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1108,7 +1147,7 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
vault backup: 2024-11-10 19:37:50
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B20A07-66D5-4FE8-BD78-B5748ABD41CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A50F39A-13A6-4D49-B1DE-A4C1D441B063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>Role</t>
   </si>
@@ -208,6 +208,42 @@
   </si>
   <si>
     <t>Cover Letter</t>
+  </si>
+  <si>
+    <t>Video Assessment</t>
+  </si>
+  <si>
+    <t>Economics Grad</t>
+  </si>
+  <si>
+    <t>https://www.efinancialcareers.co.uk/jobs-UK-London-Graduate_Economist__Macro_Economic_Research_Analyst_FTC.id20380586?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+  </si>
+  <si>
+    <t>Non-disclosed</t>
+  </si>
+  <si>
+    <t>Commercial Analyst</t>
+  </si>
+  <si>
+    <t>NESO</t>
+  </si>
+  <si>
+    <t>Wokingham</t>
+  </si>
+  <si>
+    <t>https://career4.successfactors.com/portalcareer?_s.crb=%252bAUTzxp%252fgzPJ7RjoJ%252bZdjbxTQTv%252beFevgVnAES8ceC4%253d</t>
+  </si>
+  <si>
+    <t>https://frontiereconomics.wd3.myworkdayjobs.com/en-US/Frontier_Economics_Careers/job/London/XMLNAME-2025-Undergraduate-Economic-Analyst---London_JR10075?APPLICANT_SOURCE-3-48</t>
+  </si>
+  <si>
+    <t>Frontier Economics</t>
+  </si>
+  <si>
+    <t>https://agilityresourcing.co.uk/vacancy/id/2223</t>
+  </si>
+  <si>
+    <t>Rolling</t>
   </si>
 </sst>
 </file>
@@ -746,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB83AAD-773A-4D2C-A53F-9AF66BB57483}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +797,7 @@
     <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -808,7 +844,7 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
@@ -831,8 +867,8 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F16" ca="1" si="0">C3-TODAY()</f>
-        <v>0</v>
+        <f t="shared" ref="F3:F25" ca="1" si="0">C3-TODAY()</f>
+        <v>-7</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
@@ -856,7 +892,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
@@ -880,7 +916,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
@@ -904,7 +940,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
@@ -928,7 +964,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
@@ -952,7 +988,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
@@ -976,7 +1012,7 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-14</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>28</v>
@@ -1000,34 +1036,37 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="18">
         <v>45657</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,7 +1077,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="18">
-        <v>45607</v>
+        <v>45610</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>43</v>
@@ -1048,13 +1087,13 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,7 +1114,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
@@ -1099,7 +1138,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>28</v>
@@ -1112,18 +1151,14 @@
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="2">
-        <v>45607</v>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>28</v>
@@ -1136,8 +1171,8 @@
       <c r="B16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="2">
-        <v>45607</v>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>54</v>
@@ -1145,12 +1180,146 @@
       <c r="E16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
       <c r="G16" s="8" t="s">
         <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="18">
+        <v>45608</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45610</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45625</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45610</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45606</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45606</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45606</v>
       </c>
     </row>
   </sheetData>
@@ -1196,6 +1365,10 @@
     <hyperlink ref="D14" r:id="rId13" xr:uid="{DE809EF5-F9B9-46FF-8BE7-46E61D80A9D6}"/>
     <hyperlink ref="D15" r:id="rId14" display="https://carriere.talan.com/offre-emploi/detail/?tx_talansmartrecruitorconnector_pi1%5Bid%5D=744000017588760&amp;tx_talansmartrecruitorconnector_pi1%5Baction%5D=job&amp;tx_talansmartrecruitorconnector_pi1%5Bcontroller%5D=JobOffers&amp;cHash=e6d85c147b4d326f4ed93ee51be9aa10" xr:uid="{E941F7B3-08E1-4FA5-BAF4-6DA62A0A82F7}"/>
     <hyperlink ref="D16" r:id="rId15" xr:uid="{824C8599-388D-47F0-A615-C4F85FD1051F}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{C5559029-E745-403B-9CF6-E4EB810B5C12}"/>
+    <hyperlink ref="D19" r:id="rId17" xr:uid="{F29E93A2-5DCD-48F4-A3AB-3B1070F34358}"/>
+    <hyperlink ref="D18" r:id="rId18" xr:uid="{39D0B9F3-4B1F-4AB3-80BA-21CCA41487F7}"/>
+    <hyperlink ref="D17" r:id="rId19" xr:uid="{FB1C067B-2398-47F7-9E74-CB920844D868}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2024-11-12 11:57:40
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A50F39A-13A6-4D49-B1DE-A4C1D441B063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15910A01-F3DA-4690-9D6E-26F13A5D9796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB83AAD-773A-4D2C-A53F-9AF66BB57483}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,21 +969,24 @@
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>45614</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F8">
@@ -1043,19 +1046,19 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="15">
         <v>45657</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F11">
@@ -1188,19 +1191,19 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="15">
         <v>45608</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F17">

</xml_diff>

<commit_message>
vault backup: 2024-11-15 03:57:31
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15910A01-F3DA-4690-9D6E-26F13A5D9796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4BCA1A-BDC2-4966-BE1D-FFE9CDCD3E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Role</t>
   </si>
@@ -238,9 +239,6 @@
   </si>
   <si>
     <t>Frontier Economics</t>
-  </si>
-  <si>
-    <t>https://agilityresourcing.co.uk/vacancy/id/2223</t>
   </si>
   <si>
     <t>Rolling</t>
@@ -302,7 +300,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,7 +783,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +842,7 @@
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
@@ -868,7 +866,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F25" ca="1" si="0">C3-TODAY()</f>
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
@@ -892,7 +890,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
@@ -916,7 +914,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
@@ -940,7 +938,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
@@ -964,7 +962,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
@@ -991,7 +989,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
@@ -1015,31 +1013,31 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="15">
         <v>45611</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
@@ -1063,7 +1061,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
@@ -1090,7 +1088,7 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>29</v>
@@ -1117,7 +1115,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
@@ -1141,7 +1139,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>28</v>
@@ -1155,7 +1153,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>50</v>
@@ -1175,7 +1173,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>54</v>
@@ -1208,7 +1206,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>28</v>
@@ -1218,24 +1216,24 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="10">
         <v>45610</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="9" t="s">
         <v>64</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>28</v>
@@ -1262,67 +1260,43 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="2">
-        <v>45610</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>-45606</v>
+        <v>-45610</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>-45606</v>
+        <v>-45610</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>-45606</v>
+        <v>-45610</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>-45606</v>
+        <v>-45610</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>-45606</v>
+        <v>-45610</v>
       </c>
     </row>
   </sheetData>
@@ -1368,10 +1342,9 @@
     <hyperlink ref="D14" r:id="rId13" xr:uid="{DE809EF5-F9B9-46FF-8BE7-46E61D80A9D6}"/>
     <hyperlink ref="D15" r:id="rId14" display="https://carriere.talan.com/offre-emploi/detail/?tx_talansmartrecruitorconnector_pi1%5Bid%5D=744000017588760&amp;tx_talansmartrecruitorconnector_pi1%5Baction%5D=job&amp;tx_talansmartrecruitorconnector_pi1%5Bcontroller%5D=JobOffers&amp;cHash=e6d85c147b4d326f4ed93ee51be9aa10" xr:uid="{E941F7B3-08E1-4FA5-BAF4-6DA62A0A82F7}"/>
     <hyperlink ref="D16" r:id="rId15" xr:uid="{824C8599-388D-47F0-A615-C4F85FD1051F}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{C5559029-E745-403B-9CF6-E4EB810B5C12}"/>
-    <hyperlink ref="D19" r:id="rId17" xr:uid="{F29E93A2-5DCD-48F4-A3AB-3B1070F34358}"/>
-    <hyperlink ref="D18" r:id="rId18" xr:uid="{39D0B9F3-4B1F-4AB3-80BA-21CCA41487F7}"/>
-    <hyperlink ref="D17" r:id="rId19" xr:uid="{FB1C067B-2398-47F7-9E74-CB920844D868}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{F29E93A2-5DCD-48F4-A3AB-3B1070F34358}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{39D0B9F3-4B1F-4AB3-80BA-21CCA41487F7}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{FB1C067B-2398-47F7-9E74-CB920844D868}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2024-11-20 08:04:06
</commit_message>
<xml_diff>
--- a/Extra Files/gradrolesxlsx.xlsx
+++ b/Extra Files/gradrolesxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Extra Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4BCA1A-BDC2-4966-BE1D-FFE9CDCD3E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C47EBA6-8D96-46BC-8C01-1F9684B12350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4175E2F-3864-4931-A0E4-7B18302C8A63}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>Role</t>
   </si>
@@ -242,6 +241,12 @@
   </si>
   <si>
     <t>Rolling</t>
+  </si>
+  <si>
+    <t>https://eoff.fa.em1.ukg.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_3001/job/670</t>
+  </si>
+  <si>
+    <t>Postgraduate Intern</t>
   </si>
 </sst>
 </file>
@@ -783,7 +788,8 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,24 +831,24 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="10">
         <v>45613</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F2">
         <f ca="1">C2-TODAY()</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>28</v>
@@ -866,7 +872,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F25" ca="1" si="0">C3-TODAY()</f>
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>28</v>
@@ -890,31 +896,31 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="18">
         <v>45599</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
@@ -938,31 +944,31 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="18">
         <v>45614</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>29</v>
@@ -989,7 +995,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
@@ -1013,7 +1019,7 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>-18</v>
+        <v>-22</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>28</v>
@@ -1037,7 +1043,7 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>28</v>
@@ -1061,7 +1067,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
@@ -1088,7 +1094,7 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>29</v>
@@ -1115,7 +1121,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>29</v>
@@ -1139,7 +1145,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>28</v>
@@ -1206,7 +1212,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>28</v>
@@ -1233,7 +1239,7 @@
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>28</v>
@@ -1260,43 +1266,64 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45809</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>-45610</v>
+        <v>-45614</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>-45610</v>
+        <v>-45614</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>-45610</v>
+        <v>-45614</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>-45610</v>
+        <v>-45614</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>-45610</v>
+        <v>-45614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>